<commit_message>
automation using GiD customisation (in progress)
</commit_message>
<xml_diff>
--- a/GID_Test_Paramers.xlsx
+++ b/GID_Test_Paramers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\GitHub\acse-9-independent-research-project-mt5918\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F110C40C-D419-4FA6-88AC-92E918829240}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D3461B-8405-49F6-A570-69B90E49F08E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{EDE29BB9-BB14-448B-B40B-8F9F774B9AA5}"/>
   </bookViews>
@@ -693,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA94EA70-55D9-4CD8-84D3-EF17A6D6A8A5}">
   <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>